<commit_message>
control amb una sola capa VMIX
</commit_message>
<xml_diff>
--- a/TRIAL.xlsx
+++ b/TRIAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/393df9dd6a409a6f/Documentos/PycharmProjects/TRIAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{92E1C7B1-A386-443D-81C8-76D596A28EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A76ED623-ECB7-4BAE-BD1B-306E25F8BFCF}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{A33E3B06-6CE5-41B4-B09C-8188A9022AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2346C24-2D4A-4E18-9F19-A7A71FD48D73}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VMIX" sheetId="10" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="231">
   <si>
     <t>PAIS</t>
   </si>
@@ -571,132 +571,6 @@
     <t>F_S4_6</t>
   </si>
   <si>
-    <t>1_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>1_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>1_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>1_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>1_PUNTS_P5</t>
-  </si>
-  <si>
-    <t>1_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P5</t>
-  </si>
-  <si>
-    <t>2_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P5</t>
-  </si>
-  <si>
-    <t>3_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>1_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>2_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>3_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>4_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P5</t>
-  </si>
-  <si>
-    <t>4_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>5_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P5</t>
-  </si>
-  <si>
-    <t>5_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>6_PUNTS_SECCIO</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P1</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P2</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P3</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P4</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P6</t>
-  </si>
-  <si>
-    <t>6_PUNTS_P5</t>
-  </si>
-  <si>
     <t>F_ABR_1</t>
   </si>
   <si>
@@ -827,13 +701,43 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>C_BANDERA</t>
+  </si>
+  <si>
+    <t>C_PAIS</t>
+  </si>
+  <si>
+    <t>C_PLAYER</t>
+  </si>
+  <si>
+    <t>C_PUNTS_SECCIO</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P1</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P2</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P3</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P4</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P5</t>
+  </si>
+  <si>
+    <t>C_PUNTS_P6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,8 +846,13 @@
       <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -971,24 +880,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1406,9 +1297,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1424,13 +1312,20 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1476,46 +1371,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2258,40 +2153,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF331FB-6507-44FD-A6EA-F2E5FBF3B259}">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:GL2"/>
+  <dimension ref="A1:FF7"/>
   <sheetViews>
-    <sheetView topLeftCell="ED1" workbookViewId="0">
-      <selection activeCell="EW2" sqref="EW2"/>
+    <sheetView tabSelected="1" topLeftCell="EN1" workbookViewId="0">
+      <selection activeCell="FF1" sqref="FF1:FF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="5" width="22.5703125" customWidth="1"/>
     <col min="19" max="21" width="15" customWidth="1"/>
+    <col min="92" max="92" width="48.5703125" customWidth="1"/>
+    <col min="93" max="93" width="46.85546875" customWidth="1"/>
     <col min="152" max="152" width="16.7109375" customWidth="1"/>
     <col min="153" max="153" width="14.5703125" customWidth="1"/>
-    <col min="166" max="166" width="11" customWidth="1"/>
-    <col min="194" max="194" width="14.85546875" customWidth="1"/>
+    <col min="162" max="162" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:194" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>37</v>
@@ -2714,154 +2610,58 @@
         <v>120</v>
       </c>
       <c r="EP1" s="71" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="EQ1" s="71" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="ER1" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="ES1" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="ET1" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="EU1" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="EV1" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="EW1" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="EX1" s="72" t="s">
+        <v>226</v>
+      </c>
+      <c r="EY1" s="72" t="s">
+        <v>227</v>
+      </c>
+      <c r="EZ1" s="72" t="s">
+        <v>228</v>
+      </c>
+      <c r="FA1" s="72" t="s">
+        <v>229</v>
+      </c>
+      <c r="FB1" s="72" t="s">
+        <v>230</v>
+      </c>
+      <c r="FC1" s="72" t="s">
         <v>221</v>
       </c>
-      <c r="ES1" s="71" t="s">
+      <c r="FD1" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="ET1" s="71" t="s">
+      <c r="FE1" s="72" t="s">
         <v>223</v>
       </c>
-      <c r="EU1" s="71" t="s">
-        <v>224</v>
-      </c>
-      <c r="EV1" s="72" t="s">
-        <v>195</v>
-      </c>
-      <c r="EW1" s="72" t="s">
-        <v>177</v>
-      </c>
-      <c r="EX1" s="72" t="s">
-        <v>178</v>
-      </c>
-      <c r="EY1" s="72" t="s">
-        <v>179</v>
-      </c>
-      <c r="EZ1" s="72" t="s">
-        <v>180</v>
-      </c>
-      <c r="FA1" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="FB1" s="72" t="s">
-        <v>182</v>
-      </c>
-      <c r="FC1" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="FD1" s="73" t="s">
-        <v>183</v>
-      </c>
-      <c r="FE1" s="73" t="s">
-        <v>184</v>
-      </c>
-      <c r="FF1" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="FG1" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="FH1" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="FI1" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="FJ1" s="71" t="s">
-        <v>197</v>
-      </c>
-      <c r="FK1" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="FL1" s="71" t="s">
-        <v>190</v>
-      </c>
-      <c r="FM1" s="71" t="s">
-        <v>191</v>
-      </c>
-      <c r="FN1" s="71" t="s">
-        <v>192</v>
-      </c>
-      <c r="FO1" s="71" t="s">
-        <v>193</v>
-      </c>
-      <c r="FP1" s="71" t="s">
-        <v>194</v>
-      </c>
-      <c r="FQ1" s="74" t="s">
-        <v>198</v>
-      </c>
-      <c r="FR1" s="74" t="s">
-        <v>199</v>
-      </c>
-      <c r="FS1" s="74" t="s">
-        <v>200</v>
-      </c>
-      <c r="FT1" s="74" t="s">
-        <v>201</v>
-      </c>
-      <c r="FU1" s="74" t="s">
-        <v>202</v>
-      </c>
-      <c r="FV1" s="74" t="s">
-        <v>203</v>
-      </c>
-      <c r="FW1" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="FX1" s="75" t="s">
-        <v>205</v>
-      </c>
-      <c r="FY1" s="75" t="s">
-        <v>206</v>
-      </c>
-      <c r="FZ1" s="75" t="s">
-        <v>207</v>
-      </c>
-      <c r="GA1" s="75" t="s">
-        <v>208</v>
-      </c>
-      <c r="GB1" s="75" t="s">
-        <v>209</v>
-      </c>
-      <c r="GC1" s="75" t="s">
-        <v>210</v>
-      </c>
-      <c r="GD1" s="75" t="s">
+      <c r="FF1" s="78" t="s">
         <v>211</v>
       </c>
-      <c r="GE1" s="70" t="s">
-        <v>212</v>
-      </c>
-      <c r="GF1" s="70" t="s">
-        <v>213</v>
-      </c>
-      <c r="GG1" s="70" t="s">
-        <v>214</v>
-      </c>
-      <c r="GH1" s="70" t="s">
-        <v>215</v>
-      </c>
-      <c r="GI1" s="70" t="s">
-        <v>216</v>
-      </c>
-      <c r="GJ1" s="70" t="s">
-        <v>218</v>
-      </c>
-      <c r="GK1" s="70" t="s">
-        <v>217</v>
-      </c>
-      <c r="GL1" s="81" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:194" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:162" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>TRIAL!N4</f>
         <v>TRIALS - MEN ELITE 26" - FINALS - START LIST</v>
@@ -3228,11 +3028,11 @@
       </c>
       <c r="CN2" t="str">
         <f>PLAYER1!F4</f>
-        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
+        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
       <c r="CO2" t="str">
         <f>PLAYER1!F5</f>
-        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
+        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
       <c r="CP2" t="str">
         <f>PLAYER1!F6</f>
@@ -3252,11 +3052,11 @@
       </c>
       <c r="CT2" t="str">
         <f>PLAYER1!E4</f>
-        <v>ESP</v>
+        <v>FRA</v>
       </c>
       <c r="CU2" t="str">
         <f>PLAYER1!E5</f>
-        <v>FRA</v>
+        <v>ESP</v>
       </c>
       <c r="CV2" t="str">
         <f>PLAYER1!E6</f>
@@ -3276,11 +3076,11 @@
       </c>
       <c r="CZ2" t="str">
         <f>PLAYER1!C4</f>
-        <v>ALEJANDRO MO</v>
+        <v>VINCENT H</v>
       </c>
       <c r="DA2" t="str">
         <f>PLAYER1!C5</f>
-        <v>VINCENT H</v>
+        <v>ALEJANDRO MO</v>
       </c>
       <c r="DB2" t="str">
         <f>PLAYER1!C6</f>
@@ -3375,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="DY2">
-        <f>PLAYER1!I5</f>
+        <f>PLAYER1!I4</f>
         <v>0</v>
       </c>
       <c r="DZ2">
@@ -3423,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="EK2">
-        <f>PLAYER1!K5</f>
+        <f>PLAYER1!K4</f>
         <v>0</v>
       </c>
       <c r="EL2">
@@ -3444,11 +3244,11 @@
       </c>
       <c r="EP2" t="str">
         <f>PLAYER1!D4</f>
-        <v>MON</v>
+        <v>HER</v>
       </c>
       <c r="EQ2" t="str">
         <f>PLAYER1!D5</f>
-        <v>HER</v>
+        <v>MON</v>
       </c>
       <c r="ER2" t="str">
         <f>PLAYER1!D6</f>
@@ -3494,154 +3294,35 @@
         <f>PLAYER1!N13</f>
         <v>-</v>
       </c>
-      <c r="FC2">
-        <f>PLAYER1!O14</f>
-        <v>0</v>
+      <c r="FC2" t="str">
+        <f>TRIAL!F5</f>
+        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
       <c r="FD2" t="str">
-        <f>PLAYER1!I14</f>
-        <v>-</v>
+        <f>TRIAL!E5</f>
+        <v>FRA</v>
       </c>
       <c r="FE2" t="str">
-        <f>PLAYER1!J14</f>
-        <v>-</v>
+        <f>TRIAL!C5</f>
+        <v>VINCENT H</v>
       </c>
       <c r="FF2" t="str">
-        <f>PLAYER1!K14</f>
-        <v>-</v>
-      </c>
-      <c r="FG2" t="str">
-        <f>PLAYER1!L14</f>
-        <v>-</v>
-      </c>
-      <c r="FH2" t="str">
-        <f>PLAYER1!M14</f>
-        <v>-</v>
-      </c>
-      <c r="FI2" t="str">
-        <f>PLAYER1!N14</f>
-        <v>-</v>
-      </c>
-      <c r="FJ2">
-        <f>PLAYER1!O15</f>
-        <v>0</v>
-      </c>
-      <c r="FK2" t="str">
-        <f>PLAYER1!I15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FL2" t="str">
-        <f>PLAYER1!J15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FM2" t="str">
-        <f>PLAYER1!K15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FN2" t="str">
-        <f>PLAYER1!L15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FO2" t="str">
-        <f>PLAYER1!M15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FP2" t="str">
-        <f>PLAYER1!N15</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FQ2">
-        <f>PLAYER1!O16</f>
-        <v>0</v>
-      </c>
-      <c r="FR2" t="str">
-        <f>PLAYER1!I16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FS2" t="str">
-        <f>PLAYER1!J16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FT2" t="str">
-        <f>PLAYER1!K16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FU2" t="str">
-        <f>PLAYER1!L16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FV2" t="str">
-        <f>PLAYER1!M16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FW2" t="str">
-        <f>PLAYER1!N16</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FX2">
-        <f>PLAYER1!O17</f>
-        <v>0</v>
-      </c>
-      <c r="FY2" t="str">
-        <f>PLAYER1!I17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="FZ2" t="str">
-        <f>PLAYER1!J17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GA2" t="str">
-        <f>PLAYER1!K17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GB2" t="str">
-        <f>PLAYER1!L17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GC2" t="str">
-        <f>PLAYER1!M17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GD2" t="str">
-        <f>PLAYER1!N17</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GE2">
-        <f>PLAYER1!O18</f>
-        <v>0</v>
-      </c>
-      <c r="GF2" t="str">
-        <f>PLAYER1!I18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GG2" t="str">
-        <f>PLAYER1!J18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GH2" t="str">
-        <f>PLAYER1!K18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GI2" t="str">
-        <f>PLAYER1!L18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GJ2" t="str">
-        <f>PLAYER1!M18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GK2" t="str">
-        <f>PLAYER1!N18</f>
-        <v xml:space="preserve"> -</v>
-      </c>
-      <c r="GL2" t="str">
         <f>TRIAL!U4</f>
         <v>#TrialVIC_2021</v>
       </c>
+    </row>
+    <row r="3" spans="1:162" x14ac:dyDescent="0.25">
+      <c r="EQ3" s="83"/>
+    </row>
+    <row r="7" spans="1:162" x14ac:dyDescent="0.25">
+      <c r="FC7" s="81"/>
+      <c r="FD7" s="81"/>
+      <c r="FE7" s="81"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3753,7 +3434,7 @@
     <row r="1" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="C2" s="88"/>
       <c r="D2" s="88"/>
@@ -3781,15 +3462,15 @@
       <c r="K3" s="85"/>
       <c r="L3" s="86"/>
       <c r="N3" s="93" t="s">
-        <v>246</v>
+        <v>204</v>
       </c>
       <c r="O3" s="94"/>
       <c r="P3" s="94"/>
       <c r="Q3" s="94"/>
       <c r="R3" s="94"/>
       <c r="S3" s="95"/>
-      <c r="U3" s="80" t="s">
-        <v>251</v>
+      <c r="U3" s="77" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -3830,7 +3511,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="96" t="s">
-        <v>248</v>
+        <v>206</v>
       </c>
       <c r="O4" s="97"/>
       <c r="P4" s="97"/>
@@ -3838,7 +3519,7 @@
       <c r="R4" s="97"/>
       <c r="S4" s="98"/>
       <c r="U4" s="57" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3849,16 +3530,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="77" t="s">
-        <v>226</v>
+        <v>186</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>184</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -3888,16 +3569,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="F6" s="77" t="s">
-        <v>235</v>
+        <v>192</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>193</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -3919,7 +3600,7 @@
         <v>530</v>
       </c>
       <c r="N6" s="93" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="O6" s="94"/>
       <c r="P6" s="94"/>
@@ -3935,16 +3616,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F7" s="77" t="s">
-        <v>226</v>
+        <v>186</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>184</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -3966,7 +3647,7 @@
         <v>520</v>
       </c>
       <c r="N7" s="96" t="s">
-        <v>245</v>
+        <v>203</v>
       </c>
       <c r="O7" s="97"/>
       <c r="P7" s="97"/>
@@ -3982,16 +3663,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="F8" s="77" t="s">
-        <v>235</v>
+        <v>192</v>
+      </c>
+      <c r="F8" s="74" t="s">
+        <v>193</v>
       </c>
       <c r="G8" s="6">
         <v>100</v>
@@ -4021,16 +3702,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="F9" s="77" t="s">
-        <v>235</v>
+        <v>192</v>
+      </c>
+      <c r="F9" s="74" t="s">
+        <v>193</v>
       </c>
       <c r="G9" s="6">
         <v>90</v>
@@ -4052,7 +3733,7 @@
         <v>490</v>
       </c>
       <c r="N9" s="93" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="O9" s="94"/>
       <c r="P9" s="94"/>
@@ -4068,16 +3749,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="F10" s="77" t="s">
-        <v>235</v>
+        <v>192</v>
+      </c>
+      <c r="F10" s="74" t="s">
+        <v>193</v>
       </c>
       <c r="G10" s="6">
         <v>120</v>
@@ -4099,7 +3780,7 @@
         <v>480</v>
       </c>
       <c r="N10" s="96" t="s">
-        <v>261</v>
+        <v>219</v>
       </c>
       <c r="O10" s="97"/>
       <c r="P10" s="97"/>
@@ -4113,7 +3794,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="77"/>
+      <c r="F11" s="74"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -4129,16 +3810,16 @@
         <v>17</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F12" s="77" t="s">
-        <v>226</v>
+        <v>186</v>
+      </c>
+      <c r="F12" s="74" t="s">
+        <v>184</v>
       </c>
       <c r="G12" s="6">
         <v>120</v>
@@ -4168,16 +3849,16 @@
         <v>28</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="F13" s="78" t="s">
-        <v>227</v>
+        <v>187</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>185</v>
       </c>
       <c r="G13" s="8">
         <v>120</v>
@@ -4202,7 +3883,7 @@
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="90" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="C16" s="91"/>
       <c r="D16" s="91"/>
@@ -4259,25 +3940,25 @@
       <c r="L17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="M17" s="82">
+      <c r="M17" s="79">
         <v>60</v>
       </c>
-      <c r="N17" s="83">
+      <c r="N17" s="80">
         <v>50</v>
       </c>
-      <c r="O17" s="83">
+      <c r="O17" s="80">
         <v>40</v>
       </c>
-      <c r="P17" s="83">
+      <c r="P17" s="80">
         <v>30</v>
       </c>
-      <c r="Q17" s="83">
+      <c r="Q17" s="80">
         <v>20</v>
       </c>
-      <c r="R17" s="83">
+      <c r="R17" s="80">
         <v>10</v>
       </c>
-      <c r="S17" s="83">
+      <c r="S17" s="80">
         <v>0</v>
       </c>
     </row>
@@ -4302,7 +3983,7 @@
         <f t="shared" si="2"/>
         <v>FRA</v>
       </c>
-      <c r="F18" s="79" t="str">
+      <c r="F18" s="76" t="str">
         <f t="shared" si="2"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
@@ -4380,7 +4061,7 @@
         <f t="shared" si="4"/>
         <v>ESP</v>
       </c>
-      <c r="F19" s="77" t="str">
+      <c r="F19" s="74" t="str">
         <f t="shared" si="4"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -4458,7 +4139,7 @@
         <f t="shared" si="4"/>
         <v>FRA</v>
       </c>
-      <c r="F20" s="77" t="str">
+      <c r="F20" s="74" t="str">
         <f t="shared" si="4"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
@@ -4536,7 +4217,7 @@
         <f t="shared" si="4"/>
         <v>ESP</v>
       </c>
-      <c r="F21" s="77" t="str">
+      <c r="F21" s="74" t="str">
         <f t="shared" si="4"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -4614,7 +4295,7 @@
         <f t="shared" si="4"/>
         <v>ESP</v>
       </c>
-      <c r="F22" s="77" t="str">
+      <c r="F22" s="74" t="str">
         <f t="shared" si="4"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -4692,7 +4373,7 @@
         <f t="shared" si="4"/>
         <v>ESP</v>
       </c>
-      <c r="F23" s="78" t="str">
+      <c r="F23" s="75" t="str">
         <f t="shared" si="4"/>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -4772,9 +4453,9 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13:G13"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,19 +4506,19 @@
     <row r="2" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67"/>
       <c r="B2" s="42"/>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
       <c r="N2" s="42"/>
       <c r="O2" s="43"/>
       <c r="P2" s="43"/>
@@ -4914,79 +4595,79 @@
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68">
-        <f>TRIAL!A6</f>
-        <v>2</v>
+        <f>TRIAL!A5</f>
+        <v>1</v>
       </c>
       <c r="B4" s="58">
-        <f>TRIAL!B6</f>
-        <v>7</v>
+        <f>TRIAL!B5</f>
+        <v>1</v>
       </c>
       <c r="C4" s="58" t="str">
-        <f>TRIAL!C6</f>
-        <v>ALEJANDRO MO</v>
+        <f>TRIAL!C5</f>
+        <v>VINCENT H</v>
       </c>
       <c r="D4" s="58" t="str">
-        <f>TRIAL!D6</f>
-        <v>MON</v>
+        <f>TRIAL!D5</f>
+        <v>HER</v>
       </c>
       <c r="E4" s="58" t="str">
-        <f>TRIAL!E6</f>
-        <v>ESP</v>
-      </c>
-      <c r="F4" s="76" t="str">
-        <f>TRIAL!F6</f>
-        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
+        <f>TRIAL!E5</f>
+        <v>FRA</v>
+      </c>
+      <c r="F4" s="73" t="str">
+        <f>TRIAL!F5</f>
+        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
       <c r="G4" s="58">
-        <f>$O$34</f>
+        <f>$O$24</f>
         <v>0</v>
       </c>
       <c r="H4" s="58">
-        <f>$O$35</f>
+        <f>$O$25</f>
         <v>0</v>
       </c>
       <c r="I4" s="58">
-        <f>$O$36</f>
+        <f>$O$26</f>
         <v>0</v>
       </c>
       <c r="J4" s="58">
-        <f>$O$37</f>
+        <f>$O$27</f>
         <v>0</v>
       </c>
       <c r="K4" s="58">
-        <f>$O$38</f>
+        <f>$O$28</f>
         <v>0</v>
       </c>
       <c r="L4" s="64">
-        <f>$O$39</f>
+        <f>$O$29</f>
         <v>0</v>
       </c>
       <c r="M4" s="58">
-        <f t="shared" ref="M4:M9" si="0">COUNTIF(G4:K4,$M$3)</f>
+        <f>COUNTIF(G4:K4,$M$3)</f>
         <v>0</v>
       </c>
       <c r="N4" s="58">
-        <f t="shared" ref="N4:N9" si="1">COUNTIF(G4:K4,$N$3)</f>
+        <f>COUNTIF(G4:K4,$N$3)</f>
         <v>0</v>
       </c>
       <c r="O4" s="58">
-        <f t="shared" ref="O4:O9" si="2">COUNTIF(G4:K4,$O$3)</f>
+        <f>COUNTIF(G4:K4,$O$3)</f>
         <v>0</v>
       </c>
       <c r="P4" s="58">
-        <f t="shared" ref="P4:P9" si="3">COUNTIF(G4:K4,$P$3)</f>
+        <f>COUNTIF(G4:K4,$P$3)</f>
         <v>0</v>
       </c>
       <c r="Q4" s="58">
-        <f t="shared" ref="Q4:Q9" si="4">COUNTIF(G4:K4,$Q$3)</f>
+        <f>COUNTIF(G4:K4,$Q$3)</f>
         <v>0</v>
       </c>
       <c r="R4" s="58">
-        <f t="shared" ref="R4:R9" si="5">COUNTIF(G4:K4,$R$3)</f>
+        <f>COUNTIF(G4:K4,$R$3)</f>
         <v>0</v>
       </c>
       <c r="S4" s="58">
-        <f t="shared" ref="S4:S9" si="6">COUNTIF(G4:K4,$S$3)</f>
+        <f>COUNTIF(G4:K4,$S$3)</f>
         <v>5</v>
       </c>
       <c r="T4" s="44"/>
@@ -4996,80 +4677,62 @@
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68">
-        <f>TRIAL!A5</f>
-        <v>1</v>
+        <f>TRIAL!A6</f>
+        <v>2</v>
       </c>
       <c r="B5" s="58">
-        <f>TRIAL!B5</f>
-        <v>1</v>
+        <f>TRIAL!B6</f>
+        <v>7</v>
       </c>
       <c r="C5" s="58" t="str">
-        <f>TRIAL!C5</f>
-        <v>VINCENT H</v>
+        <f>TRIAL!C6</f>
+        <v>ALEJANDRO MO</v>
       </c>
       <c r="D5" s="58" t="str">
-        <f>TRIAL!D5</f>
-        <v>HER</v>
+        <f>TRIAL!D6</f>
+        <v>MON</v>
       </c>
       <c r="E5" s="58" t="str">
-        <f>TRIAL!E5</f>
-        <v>FRA</v>
-      </c>
-      <c r="F5" s="76" t="str">
-        <f>TRIAL!F5</f>
-        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
-      </c>
-      <c r="G5" s="58">
-        <f>$O$24</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="58">
-        <f>$O$25</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="58">
-        <f>$O$26</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="58">
-        <f>$O$27</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="58">
-        <f>$O$28</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="64">
-        <f>$O$29</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="58">
-        <f t="shared" si="0"/>
+        <f>TRIAL!E6</f>
+        <v>ESP</v>
+      </c>
+      <c r="F5" s="73" t="str">
+        <f>TRIAL!F6</f>
+        <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="68">
+        <f>COUNTIF(G5:K5,$M$3)</f>
         <v>0</v>
       </c>
       <c r="N5" s="58">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(G5:K5,$N$3)</f>
         <v>0</v>
       </c>
       <c r="O5" s="58">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(G5:K5,$O$3)</f>
         <v>0</v>
       </c>
       <c r="P5" s="58">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(G5:K5,$P$3)</f>
         <v>0</v>
       </c>
       <c r="Q5" s="58">
-        <f t="shared" si="4"/>
+        <f>COUNTIF(G5:K5,$Q$3)</f>
         <v>0</v>
       </c>
       <c r="R5" s="58">
-        <f t="shared" si="5"/>
+        <f>COUNTIF(G5:K5,$R$3)</f>
         <v>0</v>
       </c>
       <c r="S5" s="58">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f>COUNTIF(G5:K5,$S$3)</f>
+        <v>0</v>
       </c>
       <c r="T5" s="44"/>
       <c r="U5" s="44"/>
@@ -5097,7 +4760,7 @@
         <f>TRIAL!E7</f>
         <v>FRA</v>
       </c>
-      <c r="F6" s="76" t="str">
+      <c r="F6" s="73" t="str">
         <f>TRIAL!F7</f>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</v>
       </c>
@@ -5126,31 +4789,31 @@
         <v>0</v>
       </c>
       <c r="M6" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M6:M9" si="0">COUNTIF(G6:K6,$M$3)</f>
         <v>0</v>
       </c>
       <c r="N6" s="58">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N6:N9" si="1">COUNTIF(G6:K6,$N$3)</f>
         <v>0</v>
       </c>
       <c r="O6" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="O6:O9" si="2">COUNTIF(G6:K6,$O$3)</f>
         <v>0</v>
       </c>
       <c r="P6" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="P6:P9" si="3">COUNTIF(G6:K6,$P$3)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="58">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="Q6:Q9" si="4">COUNTIF(G6:K6,$Q$3)</f>
         <v>0</v>
       </c>
       <c r="R6" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="R6:R9" si="5">COUNTIF(G6:K6,$R$3)</f>
         <v>0</v>
       </c>
       <c r="S6" s="58">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="S6:S9" si="6">COUNTIF(G6:K6,$S$3)</f>
         <v>5</v>
       </c>
       <c r="T6" s="44"/>
@@ -5179,7 +4842,7 @@
         <f>TRIAL!E8</f>
         <v>ESP</v>
       </c>
-      <c r="F7" s="76" t="str">
+      <c r="F7" s="73" t="str">
         <f>TRIAL!F8</f>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -5261,7 +4924,7 @@
         <f>TRIAL!E9</f>
         <v>ESP</v>
       </c>
-      <c r="F8" s="76" t="str">
+      <c r="F8" s="73" t="str">
         <f>TRIAL!F9</f>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -5343,7 +5006,7 @@
         <f>TRIAL!E10</f>
         <v>ESP</v>
       </c>
-      <c r="F9" s="76" t="str">
+      <c r="F9" s="73" t="str">
         <f>TRIAL!F10</f>
         <v>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</v>
       </c>
@@ -5498,11 +5161,11 @@
       <c r="B13" s="42"/>
       <c r="C13" s="47"/>
       <c r="D13" s="47"/>
-      <c r="E13" s="110" t="s">
+      <c r="E13" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
       <c r="H13" s="47" t="str">
         <f>TRIAL!C5</f>
         <v>VINCENT H</v>
@@ -5826,25 +5489,25 @@
         <f>TRIAL!A5</f>
         <v>1</v>
       </c>
-      <c r="C21" s="99" t="str">
+      <c r="C21" s="107" t="str">
         <f>TRIAL!C5</f>
         <v>VINCENT H</v>
       </c>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99">
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107">
         <f>TRIAL!B5</f>
         <v>1</v>
       </c>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99" t="str">
+      <c r="J21" s="107"/>
+      <c r="K21" s="107" t="str">
         <f>TRIAL!E5</f>
         <v>FRA</v>
       </c>
-      <c r="L21" s="99"/>
+      <c r="L21" s="107"/>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
@@ -5853,60 +5516,60 @@
     </row>
     <row r="22" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="22"/>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="101"/>
-      <c r="E22" s="100" t="s">
+      <c r="D22" s="100"/>
+      <c r="E22" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="100" t="s">
+      <c r="F22" s="100"/>
+      <c r="G22" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="101"/>
-      <c r="I22" s="100" t="s">
+      <c r="H22" s="100"/>
+      <c r="I22" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="101"/>
-      <c r="K22" s="100" t="s">
+      <c r="J22" s="100"/>
+      <c r="K22" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="101"/>
-      <c r="M22" s="106" t="s">
+      <c r="L22" s="100"/>
+      <c r="M22" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="101"/>
+      <c r="N22" s="100"/>
       <c r="O22" s="33"/>
       <c r="P22" s="21"/>
       <c r="U22"/>
     </row>
     <row r="23" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="22"/>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="101"/>
-      <c r="E23" s="100" t="s">
+      <c r="D23" s="100"/>
+      <c r="E23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="101"/>
-      <c r="G23" s="100" t="s">
+      <c r="F23" s="100"/>
+      <c r="G23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="101"/>
-      <c r="I23" s="100" t="s">
+      <c r="H23" s="100"/>
+      <c r="I23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="101"/>
-      <c r="K23" s="100" t="s">
+      <c r="J23" s="100"/>
+      <c r="K23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="101"/>
-      <c r="M23" s="100" t="s">
+      <c r="L23" s="100"/>
+      <c r="M23" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N23" s="101"/>
+      <c r="N23" s="100"/>
       <c r="O23" s="28" t="s">
         <v>5</v>
       </c>
@@ -5921,30 +5584,30 @@
       <c r="B24" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="D24" s="103"/>
-      <c r="E24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="F24" s="103"/>
-      <c r="G24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="H24" s="103"/>
-      <c r="I24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="J24" s="103"/>
-      <c r="K24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="L24" s="103"/>
-      <c r="M24" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="N24" s="103"/>
+      <c r="C24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="106"/>
+      <c r="E24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="F24" s="106"/>
+      <c r="G24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="H24" s="106"/>
+      <c r="I24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="J24" s="106"/>
+      <c r="K24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="L24" s="106"/>
+      <c r="M24" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="N24" s="106"/>
       <c r="O24" s="29">
         <f>_xlfn.AGGREGATE(9,6,C24:N24)</f>
         <v>0</v>
@@ -5955,30 +5618,30 @@
       <c r="B25" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="D25" s="105"/>
-      <c r="E25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="F25" s="105"/>
-      <c r="G25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="H25" s="105"/>
-      <c r="I25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="J25" s="105"/>
-      <c r="K25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="L25" s="105"/>
-      <c r="M25" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="N25" s="105"/>
+      <c r="C25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="104"/>
+      <c r="E25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="104"/>
+      <c r="G25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="H25" s="104"/>
+      <c r="I25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="J25" s="104"/>
+      <c r="K25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="L25" s="104"/>
+      <c r="M25" s="103" t="s">
+        <v>220</v>
+      </c>
+      <c r="N25" s="104"/>
       <c r="O25" s="29">
         <f t="shared" ref="O25:O28" si="7">_xlfn.AGGREGATE(9,6,C25:N25)</f>
         <v>0</v>
@@ -5989,30 +5652,30 @@
       <c r="B26" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="105"/>
-      <c r="E26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="105"/>
-      <c r="I26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="105"/>
-      <c r="K26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" s="105"/>
-      <c r="M26" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N26" s="105"/>
+      <c r="C26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="104"/>
+      <c r="E26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="104"/>
+      <c r="G26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="104"/>
+      <c r="I26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="104"/>
+      <c r="K26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="104"/>
+      <c r="M26" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="104"/>
       <c r="O26" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6023,30 +5686,30 @@
       <c r="B27" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="105"/>
-      <c r="E27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="105"/>
-      <c r="I27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="105"/>
-      <c r="K27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="105"/>
-      <c r="M27" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N27" s="105"/>
+      <c r="C27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="104"/>
+      <c r="E27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="104"/>
+      <c r="G27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="104"/>
+      <c r="I27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="104"/>
+      <c r="K27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="104"/>
+      <c r="M27" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="104"/>
       <c r="O27" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6057,30 +5720,30 @@
       <c r="B28" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="108"/>
-      <c r="G28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="108"/>
-      <c r="I28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="108"/>
-      <c r="K28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="108"/>
-      <c r="M28" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N28" s="108"/>
+      <c r="C28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="102"/>
+      <c r="E28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="102"/>
+      <c r="G28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="102"/>
+      <c r="I28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="102"/>
+      <c r="K28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="102"/>
+      <c r="M28" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="102"/>
       <c r="O28" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6113,25 +5776,25 @@
         <f>TRIAL!A6</f>
         <v>2</v>
       </c>
-      <c r="C31" s="99" t="str">
+      <c r="C31" s="107" t="str">
         <f>TRIAL!C6</f>
         <v>ALEJANDRO MO</v>
       </c>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99">
+      <c r="D31" s="107"/>
+      <c r="E31" s="107"/>
+      <c r="F31" s="107"/>
+      <c r="G31" s="107"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="107">
         <f>TRIAL!B6</f>
         <v>7</v>
       </c>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99" t="str">
+      <c r="J31" s="107"/>
+      <c r="K31" s="107" t="str">
         <f>TRIAL!E6</f>
         <v>ESP</v>
       </c>
-      <c r="L31" s="99"/>
+      <c r="L31" s="107"/>
       <c r="M31" s="32"/>
       <c r="N31" s="32"/>
       <c r="O31" s="32"/>
@@ -6139,59 +5802,59 @@
     </row>
     <row r="32" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="22"/>
-      <c r="C32" s="100" t="s">
+      <c r="C32" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="101"/>
-      <c r="E32" s="100" t="s">
+      <c r="D32" s="100"/>
+      <c r="E32" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="101"/>
-      <c r="G32" s="100" t="s">
+      <c r="F32" s="100"/>
+      <c r="G32" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="101"/>
-      <c r="I32" s="100" t="s">
+      <c r="H32" s="100"/>
+      <c r="I32" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="101"/>
-      <c r="K32" s="100" t="s">
+      <c r="J32" s="100"/>
+      <c r="K32" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L32" s="101"/>
-      <c r="M32" s="106" t="s">
+      <c r="L32" s="100"/>
+      <c r="M32" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N32" s="101"/>
+      <c r="N32" s="100"/>
       <c r="O32" s="33"/>
       <c r="P32" s="21"/>
     </row>
     <row r="33" spans="2:21" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="22"/>
-      <c r="C33" s="100" t="s">
+      <c r="C33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="101"/>
-      <c r="E33" s="100" t="s">
+      <c r="D33" s="100"/>
+      <c r="E33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="101"/>
-      <c r="G33" s="100" t="s">
+      <c r="F33" s="100"/>
+      <c r="G33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="101"/>
-      <c r="I33" s="100" t="s">
+      <c r="H33" s="100"/>
+      <c r="I33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="101"/>
-      <c r="K33" s="100" t="s">
+      <c r="J33" s="100"/>
+      <c r="K33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L33" s="101"/>
-      <c r="M33" s="100" t="s">
+      <c r="L33" s="100"/>
+      <c r="M33" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N33" s="101"/>
+      <c r="N33" s="100"/>
       <c r="O33" s="28" t="s">
         <v>5</v>
       </c>
@@ -6201,30 +5864,30 @@
       <c r="B34" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="D34" s="103"/>
-      <c r="E34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="F34" s="103"/>
-      <c r="G34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="H34" s="103"/>
-      <c r="I34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="J34" s="103"/>
-      <c r="K34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="L34" s="103"/>
-      <c r="M34" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="N34" s="103"/>
+      <c r="C34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" s="106"/>
+      <c r="E34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" s="106"/>
+      <c r="G34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="H34" s="106"/>
+      <c r="I34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="J34" s="106"/>
+      <c r="K34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="L34" s="106"/>
+      <c r="M34" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="N34" s="106"/>
       <c r="O34" s="29">
         <f>_xlfn.AGGREGATE(9,6,C34:N34)</f>
         <v>0</v>
@@ -6235,30 +5898,30 @@
       <c r="B35" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="105"/>
-      <c r="E35" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="105"/>
-      <c r="G35" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="105"/>
-      <c r="I35" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="105"/>
-      <c r="K35" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="105"/>
-      <c r="M35" s="111" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="112"/>
+      <c r="C35" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="104"/>
+      <c r="E35" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="104"/>
+      <c r="G35" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="104"/>
+      <c r="I35" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="104"/>
+      <c r="K35" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="104"/>
+      <c r="M35" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" s="109"/>
       <c r="O35" s="29">
         <f t="shared" ref="O35:O38" si="8">_xlfn.AGGREGATE(9,6,C35:N35)</f>
         <v>0</v>
@@ -6269,30 +5932,30 @@
       <c r="B36" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="105"/>
-      <c r="E36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="105"/>
-      <c r="G36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="105"/>
-      <c r="I36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="105"/>
-      <c r="K36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" s="105"/>
-      <c r="M36" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N36" s="105"/>
+      <c r="C36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="104"/>
+      <c r="E36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="104"/>
+      <c r="G36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="104"/>
+      <c r="I36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="104"/>
+      <c r="K36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L36" s="104"/>
+      <c r="M36" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N36" s="104"/>
       <c r="O36" s="29">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -6303,30 +5966,30 @@
       <c r="B37" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="105"/>
-      <c r="E37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="105"/>
-      <c r="G37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="105"/>
-      <c r="I37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="105"/>
-      <c r="K37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37" s="105"/>
-      <c r="M37" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N37" s="105"/>
+      <c r="C37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="104"/>
+      <c r="E37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="104"/>
+      <c r="G37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="104"/>
+      <c r="I37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="104"/>
+      <c r="K37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L37" s="104"/>
+      <c r="M37" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="104"/>
       <c r="O37" s="29">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -6337,30 +6000,30 @@
       <c r="B38" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="108"/>
-      <c r="E38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="108"/>
-      <c r="G38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="108"/>
-      <c r="I38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="108"/>
-      <c r="K38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L38" s="108"/>
-      <c r="M38" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N38" s="108"/>
+      <c r="C38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="102"/>
+      <c r="E38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="102"/>
+      <c r="G38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="102"/>
+      <c r="I38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="102"/>
+      <c r="K38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="102"/>
+      <c r="M38" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N38" s="102"/>
       <c r="O38" s="29">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -6393,25 +6056,25 @@
         <f>TRIAL!A7</f>
         <v>3</v>
       </c>
-      <c r="C41" s="99" t="str">
+      <c r="C41" s="107" t="str">
         <f>TRIAL!C7</f>
         <v>NICOLAS V</v>
       </c>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99">
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107">
         <f>TRIAL!B7</f>
         <v>5</v>
       </c>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99" t="str">
+      <c r="J41" s="107"/>
+      <c r="K41" s="107" t="str">
         <f>TRIAL!E7</f>
         <v>FRA</v>
       </c>
-      <c r="L41" s="99"/>
+      <c r="L41" s="107"/>
       <c r="M41" s="32"/>
       <c r="N41" s="32"/>
       <c r="O41" s="32"/>
@@ -6420,59 +6083,59 @@
     </row>
     <row r="42" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="22"/>
-      <c r="C42" s="100" t="s">
+      <c r="C42" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="101"/>
-      <c r="E42" s="100" t="s">
+      <c r="D42" s="100"/>
+      <c r="E42" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="101"/>
-      <c r="G42" s="100" t="s">
+      <c r="F42" s="100"/>
+      <c r="G42" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="101"/>
-      <c r="I42" s="100" t="s">
+      <c r="H42" s="100"/>
+      <c r="I42" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="101"/>
-      <c r="K42" s="100" t="s">
+      <c r="J42" s="100"/>
+      <c r="K42" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L42" s="101"/>
-      <c r="M42" s="106" t="s">
+      <c r="L42" s="100"/>
+      <c r="M42" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N42" s="101"/>
+      <c r="N42" s="100"/>
       <c r="O42" s="33"/>
       <c r="P42" s="21"/>
     </row>
     <row r="43" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="22"/>
-      <c r="C43" s="100" t="s">
+      <c r="C43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="100" t="s">
+      <c r="D43" s="100"/>
+      <c r="E43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="100" t="s">
+      <c r="F43" s="100"/>
+      <c r="G43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="101"/>
-      <c r="I43" s="100" t="s">
+      <c r="H43" s="100"/>
+      <c r="I43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J43" s="101"/>
-      <c r="K43" s="100" t="s">
+      <c r="J43" s="100"/>
+      <c r="K43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L43" s="101"/>
-      <c r="M43" s="100" t="s">
+      <c r="L43" s="100"/>
+      <c r="M43" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N43" s="101"/>
+      <c r="N43" s="100"/>
       <c r="O43" s="28" t="s">
         <v>5</v>
       </c>
@@ -6482,30 +6145,30 @@
       <c r="B44" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="103"/>
-      <c r="E44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="103"/>
-      <c r="G44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="103"/>
-      <c r="I44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="103"/>
-      <c r="K44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="103"/>
-      <c r="M44" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="N44" s="103"/>
+      <c r="C44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="106"/>
+      <c r="E44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="106"/>
+      <c r="G44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="106"/>
+      <c r="I44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="106"/>
+      <c r="K44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="L44" s="106"/>
+      <c r="M44" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="N44" s="106"/>
       <c r="O44" s="29">
         <f>_xlfn.AGGREGATE(9,6,C44:N44)</f>
         <v>0</v>
@@ -6516,30 +6179,30 @@
       <c r="B45" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="105"/>
-      <c r="E45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="105"/>
-      <c r="G45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="105"/>
-      <c r="I45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="105"/>
-      <c r="K45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L45" s="105"/>
-      <c r="M45" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N45" s="105"/>
+      <c r="C45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="104"/>
+      <c r="E45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="104"/>
+      <c r="G45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="104"/>
+      <c r="I45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="104"/>
+      <c r="K45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L45" s="104"/>
+      <c r="M45" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N45" s="104"/>
       <c r="O45" s="29">
         <f t="shared" ref="O45:O48" si="9">_xlfn.AGGREGATE(9,6,C45:N45)</f>
         <v>0</v>
@@ -6550,30 +6213,30 @@
       <c r="B46" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="105"/>
-      <c r="E46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="105"/>
-      <c r="G46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="105"/>
-      <c r="I46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="105"/>
-      <c r="K46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L46" s="105"/>
-      <c r="M46" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N46" s="105"/>
+      <c r="C46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="104"/>
+      <c r="E46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="104"/>
+      <c r="G46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="104"/>
+      <c r="I46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="104"/>
+      <c r="K46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46" s="104"/>
+      <c r="M46" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N46" s="104"/>
       <c r="O46" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6584,30 +6247,30 @@
       <c r="B47" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="105"/>
-      <c r="E47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="105"/>
-      <c r="G47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47" s="105"/>
-      <c r="I47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="105"/>
-      <c r="K47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L47" s="105"/>
-      <c r="M47" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N47" s="105"/>
+      <c r="C47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="104"/>
+      <c r="E47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="104"/>
+      <c r="G47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="104"/>
+      <c r="I47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="104"/>
+      <c r="K47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47" s="104"/>
+      <c r="M47" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N47" s="104"/>
       <c r="O47" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6618,30 +6281,30 @@
       <c r="B48" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="108"/>
-      <c r="E48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="108"/>
-      <c r="G48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="108"/>
-      <c r="I48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="108"/>
-      <c r="K48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L48" s="108"/>
-      <c r="M48" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N48" s="108"/>
+      <c r="C48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="102"/>
+      <c r="E48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="102"/>
+      <c r="G48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="102"/>
+      <c r="I48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" s="102"/>
+      <c r="K48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48" s="102"/>
+      <c r="M48" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N48" s="102"/>
       <c r="O48" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6689,25 +6352,25 @@
         <f>TRIAL!A8</f>
         <v>4</v>
       </c>
-      <c r="C51" s="99" t="str">
+      <c r="C51" s="107" t="str">
         <f>TRIAL!C8</f>
         <v>BORJA CO</v>
       </c>
-      <c r="D51" s="99"/>
-      <c r="E51" s="99"/>
-      <c r="F51" s="99"/>
-      <c r="G51" s="99"/>
-      <c r="H51" s="99"/>
-      <c r="I51" s="99">
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="107"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107">
         <f>TRIAL!B8</f>
         <v>6</v>
       </c>
-      <c r="J51" s="99"/>
-      <c r="K51" s="99" t="str">
+      <c r="J51" s="107"/>
+      <c r="K51" s="107" t="str">
         <f>TRIAL!E8</f>
         <v>ESP</v>
       </c>
-      <c r="L51" s="99"/>
+      <c r="L51" s="107"/>
       <c r="M51" s="32"/>
       <c r="N51" s="32"/>
       <c r="O51" s="32"/>
@@ -6715,59 +6378,59 @@
     </row>
     <row r="52" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="22"/>
-      <c r="C52" s="100" t="s">
+      <c r="C52" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="101"/>
-      <c r="E52" s="100" t="s">
+      <c r="D52" s="100"/>
+      <c r="E52" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="101"/>
-      <c r="G52" s="100" t="s">
+      <c r="F52" s="100"/>
+      <c r="G52" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="101"/>
-      <c r="I52" s="100" t="s">
+      <c r="H52" s="100"/>
+      <c r="I52" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J52" s="101"/>
-      <c r="K52" s="100" t="s">
+      <c r="J52" s="100"/>
+      <c r="K52" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L52" s="101"/>
-      <c r="M52" s="106" t="s">
+      <c r="L52" s="100"/>
+      <c r="M52" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N52" s="101"/>
+      <c r="N52" s="100"/>
       <c r="O52" s="33"/>
       <c r="P52" s="21"/>
     </row>
     <row r="53" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="22"/>
-      <c r="C53" s="100" t="s">
+      <c r="C53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="101"/>
-      <c r="E53" s="100" t="s">
+      <c r="D53" s="100"/>
+      <c r="E53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="101"/>
-      <c r="G53" s="100" t="s">
+      <c r="F53" s="100"/>
+      <c r="G53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="101"/>
-      <c r="I53" s="100" t="s">
+      <c r="H53" s="100"/>
+      <c r="I53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="101"/>
-      <c r="K53" s="100" t="s">
+      <c r="J53" s="100"/>
+      <c r="K53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L53" s="101"/>
-      <c r="M53" s="100" t="s">
+      <c r="L53" s="100"/>
+      <c r="M53" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N53" s="101"/>
+      <c r="N53" s="100"/>
       <c r="O53" s="28" t="s">
         <v>5</v>
       </c>
@@ -6777,30 +6440,30 @@
       <c r="B54" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="103"/>
-      <c r="E54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="103"/>
-      <c r="G54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="H54" s="103"/>
-      <c r="I54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="103"/>
-      <c r="K54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="L54" s="103"/>
-      <c r="M54" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="N54" s="103"/>
+      <c r="C54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="106"/>
+      <c r="E54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="106"/>
+      <c r="G54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="106"/>
+      <c r="I54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="106"/>
+      <c r="K54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="L54" s="106"/>
+      <c r="M54" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="106"/>
       <c r="O54" s="29">
         <f>_xlfn.AGGREGATE(9,6,C54:N54)</f>
         <v>0</v>
@@ -6811,30 +6474,30 @@
       <c r="B55" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="105"/>
-      <c r="E55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" s="105"/>
-      <c r="G55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="105"/>
-      <c r="I55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="105"/>
-      <c r="K55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L55" s="105"/>
-      <c r="M55" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N55" s="105"/>
+      <c r="C55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="104"/>
+      <c r="E55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="104"/>
+      <c r="G55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="104"/>
+      <c r="I55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="104"/>
+      <c r="K55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L55" s="104"/>
+      <c r="M55" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N55" s="104"/>
       <c r="O55" s="29">
         <f t="shared" ref="O55:O58" si="10">_xlfn.AGGREGATE(9,6,C55:N55)</f>
         <v>0</v>
@@ -6845,30 +6508,30 @@
       <c r="B56" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="105"/>
-      <c r="E56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="105"/>
-      <c r="G56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" s="105"/>
-      <c r="I56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J56" s="105"/>
-      <c r="K56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L56" s="105"/>
-      <c r="M56" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N56" s="105"/>
+      <c r="C56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="104"/>
+      <c r="E56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="104"/>
+      <c r="G56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="104"/>
+      <c r="I56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="104"/>
+      <c r="K56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L56" s="104"/>
+      <c r="M56" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N56" s="104"/>
       <c r="O56" s="29">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -6879,30 +6542,30 @@
       <c r="B57" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="105"/>
-      <c r="E57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F57" s="105"/>
-      <c r="G57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H57" s="105"/>
-      <c r="I57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="105"/>
-      <c r="K57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L57" s="105"/>
-      <c r="M57" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N57" s="105"/>
+      <c r="C57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="104"/>
+      <c r="E57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="104"/>
+      <c r="G57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="104"/>
+      <c r="I57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="104"/>
+      <c r="K57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L57" s="104"/>
+      <c r="M57" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" s="104"/>
       <c r="O57" s="29">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -6913,30 +6576,30 @@
       <c r="B58" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="108"/>
-      <c r="E58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" s="108"/>
-      <c r="G58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H58" s="108"/>
-      <c r="I58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="108"/>
-      <c r="K58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L58" s="108"/>
-      <c r="M58" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N58" s="108"/>
+      <c r="C58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="102"/>
+      <c r="E58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="102"/>
+      <c r="G58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="102"/>
+      <c r="I58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="102"/>
+      <c r="K58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L58" s="102"/>
+      <c r="M58" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N58" s="102"/>
       <c r="O58" s="29">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -6969,25 +6632,25 @@
         <f>TRIAL!A9</f>
         <v>5</v>
       </c>
-      <c r="C61" s="99" t="str">
+      <c r="C61" s="107" t="str">
         <f>TRIAL!C9</f>
         <v>ELOI PA</v>
       </c>
-      <c r="D61" s="99"/>
-      <c r="E61" s="99"/>
-      <c r="F61" s="99"/>
-      <c r="G61" s="99"/>
-      <c r="H61" s="99"/>
-      <c r="I61" s="99">
+      <c r="D61" s="107"/>
+      <c r="E61" s="107"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="107"/>
+      <c r="H61" s="107"/>
+      <c r="I61" s="107">
         <f>TRIAL!B9</f>
         <v>4</v>
       </c>
-      <c r="J61" s="99"/>
-      <c r="K61" s="99" t="str">
+      <c r="J61" s="107"/>
+      <c r="K61" s="107" t="str">
         <f>TRIAL!E9</f>
         <v>ESP</v>
       </c>
-      <c r="L61" s="99"/>
+      <c r="L61" s="107"/>
       <c r="M61" s="32"/>
       <c r="N61" s="32"/>
       <c r="O61" s="32"/>
@@ -6995,59 +6658,59 @@
     </row>
     <row r="62" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="22"/>
-      <c r="C62" s="100" t="s">
+      <c r="C62" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D62" s="101"/>
-      <c r="E62" s="100" t="s">
+      <c r="D62" s="100"/>
+      <c r="E62" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="101"/>
-      <c r="G62" s="100" t="s">
+      <c r="F62" s="100"/>
+      <c r="G62" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H62" s="101"/>
-      <c r="I62" s="100" t="s">
+      <c r="H62" s="100"/>
+      <c r="I62" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J62" s="101"/>
-      <c r="K62" s="100" t="s">
+      <c r="J62" s="100"/>
+      <c r="K62" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L62" s="101"/>
-      <c r="M62" s="106" t="s">
+      <c r="L62" s="100"/>
+      <c r="M62" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N62" s="101"/>
+      <c r="N62" s="100"/>
       <c r="O62" s="33"/>
       <c r="P62" s="21"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="22"/>
-      <c r="C63" s="100" t="s">
+      <c r="C63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="101"/>
-      <c r="E63" s="100" t="s">
+      <c r="D63" s="100"/>
+      <c r="E63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="101"/>
-      <c r="G63" s="100" t="s">
+      <c r="F63" s="100"/>
+      <c r="G63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H63" s="101"/>
-      <c r="I63" s="100" t="s">
+      <c r="H63" s="100"/>
+      <c r="I63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J63" s="101"/>
-      <c r="K63" s="100" t="s">
+      <c r="J63" s="100"/>
+      <c r="K63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L63" s="101"/>
-      <c r="M63" s="100" t="s">
+      <c r="L63" s="100"/>
+      <c r="M63" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N63" s="101"/>
+      <c r="N63" s="100"/>
       <c r="O63" s="28" t="s">
         <v>5</v>
       </c>
@@ -7057,30 +6720,30 @@
       <c r="B64" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="103"/>
-      <c r="E64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F64" s="103"/>
-      <c r="G64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="H64" s="103"/>
-      <c r="I64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="J64" s="103"/>
-      <c r="K64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="L64" s="103"/>
-      <c r="M64" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="N64" s="103"/>
+      <c r="C64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="106"/>
+      <c r="E64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="106"/>
+      <c r="G64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="106"/>
+      <c r="I64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="106"/>
+      <c r="K64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="L64" s="106"/>
+      <c r="M64" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="N64" s="106"/>
       <c r="O64" s="29">
         <f>_xlfn.AGGREGATE(9,6,C64:N64)</f>
         <v>0</v>
@@ -7091,30 +6754,30 @@
       <c r="B65" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="105"/>
-      <c r="E65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="105"/>
-      <c r="G65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H65" s="105"/>
-      <c r="I65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J65" s="105"/>
-      <c r="K65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L65" s="105"/>
-      <c r="M65" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N65" s="105"/>
+      <c r="C65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="104"/>
+      <c r="E65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="104"/>
+      <c r="G65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="104"/>
+      <c r="I65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="104"/>
+      <c r="K65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L65" s="104"/>
+      <c r="M65" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N65" s="104"/>
       <c r="O65" s="29">
         <f t="shared" ref="O65:O68" si="11">_xlfn.AGGREGATE(9,6,C65:N65)</f>
         <v>0</v>
@@ -7125,30 +6788,30 @@
       <c r="B66" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="105"/>
-      <c r="E66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="105"/>
-      <c r="G66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" s="105"/>
-      <c r="I66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" s="105"/>
-      <c r="K66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L66" s="105"/>
-      <c r="M66" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N66" s="105"/>
+      <c r="C66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="104"/>
+      <c r="E66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="104"/>
+      <c r="G66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="104"/>
+      <c r="I66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="104"/>
+      <c r="K66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L66" s="104"/>
+      <c r="M66" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N66" s="104"/>
       <c r="O66" s="29">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -7159,30 +6822,30 @@
       <c r="B67" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="105"/>
-      <c r="E67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="105"/>
-      <c r="G67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" s="105"/>
-      <c r="I67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J67" s="105"/>
-      <c r="K67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L67" s="105"/>
-      <c r="M67" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N67" s="105"/>
+      <c r="C67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="104"/>
+      <c r="E67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="104"/>
+      <c r="G67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="104"/>
+      <c r="I67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" s="104"/>
+      <c r="K67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L67" s="104"/>
+      <c r="M67" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N67" s="104"/>
       <c r="O67" s="29">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -7193,30 +6856,30 @@
       <c r="B68" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="108"/>
-      <c r="E68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="108"/>
-      <c r="G68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" s="108"/>
-      <c r="I68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J68" s="108"/>
-      <c r="K68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L68" s="108"/>
-      <c r="M68" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N68" s="108"/>
+      <c r="C68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="102"/>
+      <c r="E68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="102"/>
+      <c r="G68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="102"/>
+      <c r="I68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J68" s="102"/>
+      <c r="K68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L68" s="102"/>
+      <c r="M68" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N68" s="102"/>
       <c r="O68" s="29">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -7249,25 +6912,25 @@
         <f>TRIAL!A10</f>
         <v>6</v>
       </c>
-      <c r="C71" s="99" t="str">
+      <c r="C71" s="107" t="str">
         <f>TRIAL!C10</f>
         <v>JULEN S</v>
       </c>
-      <c r="D71" s="99"/>
-      <c r="E71" s="99"/>
-      <c r="F71" s="99"/>
-      <c r="G71" s="99"/>
-      <c r="H71" s="99"/>
-      <c r="I71" s="99">
+      <c r="D71" s="107"/>
+      <c r="E71" s="107"/>
+      <c r="F71" s="107"/>
+      <c r="G71" s="107"/>
+      <c r="H71" s="107"/>
+      <c r="I71" s="107">
         <f>TRIAL!B10</f>
         <v>9</v>
       </c>
-      <c r="J71" s="99"/>
-      <c r="K71" s="99" t="str">
+      <c r="J71" s="107"/>
+      <c r="K71" s="107" t="str">
         <f>TRIAL!E10</f>
         <v>ESP</v>
       </c>
-      <c r="L71" s="99"/>
+      <c r="L71" s="107"/>
       <c r="M71" s="32"/>
       <c r="N71" s="32"/>
       <c r="O71" s="32"/>
@@ -7275,59 +6938,59 @@
     </row>
     <row r="72" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="22"/>
-      <c r="C72" s="100" t="s">
+      <c r="C72" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="101"/>
-      <c r="E72" s="100" t="s">
+      <c r="D72" s="100"/>
+      <c r="E72" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F72" s="101"/>
-      <c r="G72" s="100" t="s">
+      <c r="F72" s="100"/>
+      <c r="G72" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="H72" s="101"/>
-      <c r="I72" s="100" t="s">
+      <c r="H72" s="100"/>
+      <c r="I72" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="J72" s="101"/>
-      <c r="K72" s="100" t="s">
+      <c r="J72" s="100"/>
+      <c r="K72" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="L72" s="101"/>
-      <c r="M72" s="106" t="s">
+      <c r="L72" s="100"/>
+      <c r="M72" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="N72" s="101"/>
+      <c r="N72" s="100"/>
       <c r="O72" s="33"/>
       <c r="P72" s="21"/>
     </row>
     <row r="73" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="22"/>
-      <c r="C73" s="100" t="s">
+      <c r="C73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="101"/>
-      <c r="E73" s="100" t="s">
+      <c r="D73" s="100"/>
+      <c r="E73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F73" s="101"/>
-      <c r="G73" s="100" t="s">
+      <c r="F73" s="100"/>
+      <c r="G73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="H73" s="101"/>
-      <c r="I73" s="100" t="s">
+      <c r="H73" s="100"/>
+      <c r="I73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="J73" s="101"/>
-      <c r="K73" s="100" t="s">
+      <c r="J73" s="100"/>
+      <c r="K73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="L73" s="101"/>
-      <c r="M73" s="100" t="s">
+      <c r="L73" s="100"/>
+      <c r="M73" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="N73" s="101"/>
+      <c r="N73" s="100"/>
       <c r="O73" s="28" t="s">
         <v>5</v>
       </c>
@@ -7337,30 +7000,30 @@
       <c r="B74" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="103"/>
-      <c r="E74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" s="103"/>
-      <c r="G74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="H74" s="103"/>
-      <c r="I74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="J74" s="103"/>
-      <c r="K74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="L74" s="103"/>
-      <c r="M74" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="N74" s="103"/>
+      <c r="C74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="106"/>
+      <c r="E74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="106"/>
+      <c r="G74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="106"/>
+      <c r="I74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J74" s="106"/>
+      <c r="K74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="L74" s="106"/>
+      <c r="M74" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="N74" s="106"/>
       <c r="O74" s="29">
         <f>_xlfn.AGGREGATE(9,6,C74:N74)</f>
         <v>0</v>
@@ -7371,30 +7034,30 @@
       <c r="B75" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="105"/>
-      <c r="E75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="105"/>
-      <c r="G75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H75" s="105"/>
-      <c r="I75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J75" s="105"/>
-      <c r="K75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L75" s="105"/>
-      <c r="M75" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N75" s="105"/>
+      <c r="C75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="104"/>
+      <c r="E75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="104"/>
+      <c r="G75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="104"/>
+      <c r="I75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75" s="104"/>
+      <c r="K75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L75" s="104"/>
+      <c r="M75" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N75" s="104"/>
       <c r="O75" s="29">
         <f t="shared" ref="O75:O78" si="12">_xlfn.AGGREGATE(9,6,C75:N75)</f>
         <v>0</v>
@@ -7405,30 +7068,30 @@
       <c r="B76" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="105"/>
-      <c r="E76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="105"/>
-      <c r="G76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H76" s="105"/>
-      <c r="I76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J76" s="105"/>
-      <c r="K76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L76" s="105"/>
-      <c r="M76" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N76" s="105"/>
+      <c r="C76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="104"/>
+      <c r="E76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="104"/>
+      <c r="G76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H76" s="104"/>
+      <c r="I76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J76" s="104"/>
+      <c r="K76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L76" s="104"/>
+      <c r="M76" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N76" s="104"/>
       <c r="O76" s="29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -7439,30 +7102,30 @@
       <c r="B77" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="105"/>
-      <c r="E77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="105"/>
-      <c r="G77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="H77" s="105"/>
-      <c r="I77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="J77" s="105"/>
-      <c r="K77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="L77" s="105"/>
-      <c r="M77" s="104" t="s">
-        <v>14</v>
-      </c>
-      <c r="N77" s="105"/>
+      <c r="C77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="104"/>
+      <c r="E77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="104"/>
+      <c r="G77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="104"/>
+      <c r="I77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="104"/>
+      <c r="K77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="L77" s="104"/>
+      <c r="M77" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="N77" s="104"/>
       <c r="O77" s="29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -7473,30 +7136,30 @@
       <c r="B78" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="108"/>
-      <c r="E78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="108"/>
-      <c r="G78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="H78" s="108"/>
-      <c r="I78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="J78" s="108"/>
-      <c r="K78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="L78" s="108"/>
-      <c r="M78" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="N78" s="108"/>
+      <c r="C78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="102"/>
+      <c r="E78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="102"/>
+      <c r="G78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="102"/>
+      <c r="I78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="J78" s="102"/>
+      <c r="K78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="L78" s="102"/>
+      <c r="M78" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N78" s="102"/>
       <c r="O78" s="29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -7525,69 +7188,191 @@
     </row>
   </sheetData>
   <mergeCells count="272">
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="M78:N78"/>
-    <mergeCell ref="M77:N77"/>
-    <mergeCell ref="M76:N76"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="K78:L78"/>
-    <mergeCell ref="K77:L77"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="M68:N68"/>
-    <mergeCell ref="M67:N67"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="C61:H61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K54:L54"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="I48:J48"/>
@@ -7612,191 +7397,69 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="M56:N56"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="C61:H61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="M77:N77"/>
+    <mergeCell ref="M76:N76"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K74:L74"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">

</xml_diff>